<commit_message>
Added PCA stress, stable rank
</commit_message>
<xml_diff>
--- a/Experiments/dimensionality_reduction_metrics/results/theoretical_optimum.xlsx
+++ b/Experiments/dimensionality_reduction_metrics/results/theoretical_optimum.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -876,6 +876,267 @@
         <v>0.1523358399849055</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2023-07-17 02:02:19</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>stress</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>10</v>
+      </c>
+      <c r="E16" t="n">
+        <v>8</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.004945099992587836</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2023-07-17 02:03:18</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>stress</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>10</v>
+      </c>
+      <c r="E17" t="n">
+        <v>8</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.004945099992587836</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2023-07-17 02:03:18</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>stress</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>7</v>
+      </c>
+      <c r="E18" t="n">
+        <v>5</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.01952064496563264</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2023-07-17 02:03:18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>stress</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.5680354784012266</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2023-07-17 02:03:18</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>stress</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>6</v>
+      </c>
+      <c r="E20" t="n">
+        <v>5</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.02760636085666775</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2023-07-17 02:03:19</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>stress</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>5</v>
+      </c>
+      <c r="E21" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.04585823797499209</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2023-07-17 02:03:19</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>stress</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>3</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.2352084552295149</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2023-07-17 02:03:19</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>stress</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>8</v>
+      </c>
+      <c r="E23" t="n">
+        <v>7</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.01383268926919492</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2023-07-17 02:03:19</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>stress</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>